<commit_message>
Commit Final - Entrega de trabalho
</commit_message>
<xml_diff>
--- a/cruzreta.xlsx
+++ b/cruzreta.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\USP\4°Semestre\Fund. Biomecânica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\USP\4°Semestre\Fund. Biomecânica\Cruzamento de retas\Cruzamento-de-retas-biomec\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -688,7 +688,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>